<commit_message>
remove some vocabulary file
</commit_message>
<xml_diff>
--- a/英语词库/词缀说文解字.xlsx
+++ b/英语词库/词缀说文解字.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="16875" windowHeight="9930"/>
+    <workbookView windowWidth="23895" windowHeight="9930"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -85,6 +85,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -92,14 +99,67 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -108,36 +168,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -153,14 +184,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -174,24 +197,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -206,14 +214,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
@@ -237,6 +237,180 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -244,180 +418,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -428,6 +428,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -461,6 +485,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -476,30 +520,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -508,26 +528,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -536,10 +536,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -548,133 +548,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>

</xml_diff>